<commit_message>
Added first Patient endpoint test scenarios and supporting steps
</commit_message>
<xml_diff>
--- a/Data/Test Suite Required Patients.xlsx
+++ b/Data/Test Suite Required Patients.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="41">
   <si>
     <t xml:space="preserve">Cells containing a '0' should not have any data for that section
 Cells containing an 'x' should have data for that section 
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t xml:space="preserve">Patient which has opted out of data sharing agreement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient with same NHS number as “Patient3”</t>
   </si>
 </sst>
 </file>
@@ -152,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -259,6 +265,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFBFBFBF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB2B2B2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -304,7 +317,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
     <fill>
@@ -455,7 +468,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -514,6 +527,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -590,7 +611,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -609,13 +630,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O13" activeCellId="0" sqref="O13"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="2" style="2" width="19.91"/>
@@ -1376,6 +1397,53 @@
         <v>38</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>

</xml_diff>

<commit_message>
Added 0.7.4 tests. Removed old traits and added new traits.
</commit_message>
<xml_diff>
--- a/Data/Test Suite Required Patients.xlsx
+++ b/Data/Test Suite Required Patients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sado1\Desktop\GP Connect notes\EMIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GPConnect\Provider\0.7.4\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7935607F-92E5-4231-82C4-FCA49A8D4955}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEAEBA0-F790-477D-A528-BE9D1E5D692B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14805" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="47">
   <si>
     <t>Administrative Items</t>
   </si>
@@ -160,6 +160,18 @@
   </si>
   <si>
     <t>Other Inactive Problems</t>
+  </si>
+  <si>
+    <t>Patient Must have deceased Datetime with in allowed access period "28" days</t>
+  </si>
+  <si>
+    <t>Patient Must have deceased Datetime over allowed access period "28" days. i.e deceased Datetime must be older than"28" days.</t>
+  </si>
+  <si>
+    <t>Patient 17</t>
+  </si>
+  <si>
+    <t>Patient 18</t>
   </si>
 </sst>
 </file>
@@ -703,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMN18"/>
+  <dimension ref="A1:AMN20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,6 +1629,118 @@
         <v>33</v>
       </c>
     </row>
+    <row r="19" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="P19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R20" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:R1"/>

</xml_diff>